<commit_message>
Teff data spreadsheet work
</commit_message>
<xml_diff>
--- a/Prototypes/Tef/TeffDataWorkings.xlsx
+++ b/Prototypes/Tef/TeffDataWorkings.xlsx
@@ -232,13 +232,14 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="8.6564274522718879E-2"/>
-                  <c:y val="0.39933175853018371"/>
+                  <c:x val="-0.4627862938235382"/>
+                  <c:y val="0.19278188976377952"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -517,11 +518,55 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="59924480"/>
-        <c:axId val="59914496"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$S$1:$S$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$U$1:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="124153216"/>
+        <c:axId val="124171776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59924480"/>
+        <c:axId val="124153216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,12 +591,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59914496"/>
+        <c:crossAx val="124171776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59914496"/>
+        <c:axId val="124171776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +622,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59924480"/>
+        <c:crossAx val="124153216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -586,10 +631,414 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-AU"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Total Biomass</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>119.49</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>167.19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>205.89</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>131.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>2197</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3170</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6894</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5177</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6700</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11500</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5719</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7904</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9392</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9652</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8038</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7620</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6220</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4630</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3930</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4530</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3480</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Yield</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>20.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>119.49</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>167.19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>205.89</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>131.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="35"/>
+                <c:pt idx="0">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1158</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1963</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2539</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2118</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3180</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2520</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2860</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2730</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2320</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3170</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2970</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2740</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2540</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3130</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2770</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2550</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2940</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2111</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2831</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3380</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3444</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2918</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1170</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>370</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="139019392"/>
+        <c:axId val="139017600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="139019392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> Crop N (kg/ha)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="139017600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="139017600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="139019392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId1"/>
 </c:chartSpace>
 </file>
 
@@ -620,6 +1069,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -664,6 +1143,91 @@
               </a:solidFill>
             </a:rPr>
             <a:t>Harvest Index = 0.4</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.64449</cdr:x>
+      <cdr:y>0.502</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.91825</cdr:x>
+      <cdr:y>0.572</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2583180" y="1912620"/>
+          <a:ext cx="1097263" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Harvest Index = 0.2</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -957,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:T38"/>
+  <dimension ref="B1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -972,15 +1536,18 @@
     <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20">
+    <row r="1" spans="2:21">
       <c r="S1">
         <v>0</v>
       </c>
       <c r="T1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="2:20">
+      <c r="U1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21">
       <c r="S2">
         <v>10000</v>
       </c>
@@ -988,8 +1555,11 @@
         <f>S2*0.4</f>
         <v>4000</v>
       </c>
-    </row>
-    <row r="3" spans="2:20">
+      <c r="U2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:20">
+    <row r="4" spans="2:21">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -1071,7 +1641,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:21">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -1109,7 +1679,7 @@
         <v>142.30000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:21">
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -1147,7 +1717,7 @@
         <v>146.30000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:20">
+    <row r="7" spans="2:21">
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -1185,7 +1755,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
+    <row r="8" spans="2:21">
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -1223,7 +1793,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:21">
       <c r="B9" t="s">
         <v>18</v>
       </c>
@@ -1245,7 +1815,7 @@
         <v>0.23571428571428571</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
+    <row r="10" spans="2:21">
       <c r="C10" t="s">
         <v>20</v>
       </c>
@@ -1264,7 +1834,7 @@
         <v>0.28392857142857142</v>
       </c>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:21">
       <c r="C11" t="s">
         <v>21</v>
       </c>
@@ -1283,7 +1853,7 @@
         <v>0.37611940298507462</v>
       </c>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:21">
       <c r="C12" t="s">
         <v>22</v>
       </c>
@@ -1302,7 +1872,7 @@
         <v>0.14666666666666667</v>
       </c>
     </row>
-    <row r="13" spans="2:20">
+    <row r="13" spans="2:21">
       <c r="C13" t="s">
         <v>23</v>
       </c>
@@ -1321,7 +1891,7 @@
         <v>0.46129032258064517</v>
       </c>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:21">
       <c r="C14" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1910,7 @@
         <v>0.3329268292682927</v>
       </c>
     </row>
-    <row r="15" spans="2:20">
+    <row r="15" spans="2:21">
       <c r="C15" t="s">
         <v>25</v>
       </c>
@@ -1359,7 +1929,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:21">
       <c r="C16" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
More work on teff validation set
</commit_message>
<xml_diff>
--- a/Prototypes/Tef/TeffDataWorkings.xlsx
+++ b/Prototypes/Tef/TeffDataWorkings.xlsx
@@ -192,8 +192,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -238,7 +239,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.4627862938235382"/>
+                  <c:x val="-0.46278629382353825"/>
                   <c:y val="0.19278188976377952"/>
                 </c:manualLayout>
               </c:layout>
@@ -562,11 +563,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="124153216"/>
-        <c:axId val="124171776"/>
+        <c:axId val="57146752"/>
+        <c:axId val="114042368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="124153216"/>
+        <c:axId val="57146752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,12 +592,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124171776"/>
+        <c:crossAx val="114042368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="124171776"/>
+        <c:axId val="114042368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -622,7 +623,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124153216"/>
+        <c:crossAx val="57146752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -631,7 +632,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -976,11 +977,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="139019392"/>
-        <c:axId val="139017600"/>
+        <c:axId val="114181632"/>
+        <c:axId val="56877056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139019392"/>
+        <c:axId val="114181632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1010,12 +1011,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139017600"/>
+        <c:crossAx val="56877056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139017600"/>
+        <c:axId val="56877056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1023,7 +1024,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139019392"/>
+        <c:crossAx val="114181632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1036,7 +1037,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1523,8 +1524,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="864" topLeftCell="A8" activePane="bottomLeft"/>
+      <selection activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1833,6 +1836,7 @@
         <f t="shared" si="1"/>
         <v>0.28392857142857142</v>
       </c>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="2:21">
       <c r="C11" t="s">
@@ -1852,6 +1856,7 @@
         <f t="shared" si="1"/>
         <v>0.37611940298507462</v>
       </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="2:21">
       <c r="C12" t="s">

</xml_diff>